<commit_message>
nog een test + logboek update
</commit_message>
<xml_diff>
--- a/Logboek voetbal.xlsx
+++ b/Logboek voetbal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="8550"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Logboek" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>2de paasdag</t>
   </si>
@@ -52,40 +52,52 @@
     <t>maken van PvA, Rolverdeling gemaakt, Github accounts aangemaakt</t>
   </si>
   <si>
-    <t>(ontwerpschets iedereen, samenwerkingscontract en bereikbaarheidslijst door Corwin)</t>
-  </si>
-  <si>
-    <t>(PvA door Yannick, Rolverdeling + GitHub accounts iedereen)</t>
-  </si>
-  <si>
-    <t>(Conventierapport door Sven)</t>
-  </si>
-  <si>
-    <t>(Voorkant door Steven</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Logboek door Steven en Yannick, verbeteren PvA door Corwin </t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
     <t>Steven, Corwin en Yannick</t>
   </si>
   <si>
-    <t>6-11 apr</t>
-  </si>
-  <si>
-    <t>Prototype door Yannick</t>
-  </si>
-  <si>
     <t>meivakantie, prototype gemaakt</t>
   </si>
   <si>
-    <t>Prototype door Yannick en Corwin, rapport database naar programma door Sven, onderzoek database verslag door Steven</t>
-  </si>
-  <si>
     <t>Prototype verder gemaakt, rapport database &gt; programma, database onderzoek verslag, flowchart</t>
+  </si>
+  <si>
+    <t>6-11 mei</t>
+  </si>
+  <si>
+    <t>ontwerpschets iedereen, samenwerkingscontract en bereikbaarheidslijst Corwin</t>
+  </si>
+  <si>
+    <t>Conventierapport door Sven</t>
+  </si>
+  <si>
+    <t>PvA Yannick, Rolverdeling + GitHub accounts iedereen</t>
+  </si>
+  <si>
+    <t>Voorkant Steven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logboek Steven en Yannick, verbeteren PvA Corwin </t>
+  </si>
+  <si>
+    <t>Prototype Yannick</t>
+  </si>
+  <si>
+    <t>Prototype Yannick en Corwin, rapport database naar programma Sven, onderzoek database verslag Steven</t>
+  </si>
+  <si>
+    <t>database verslag Steven, PvA Yannick, GitHub iedereen</t>
+  </si>
+  <si>
+    <t>Onderzoek database verslag verder, PvA aangepast, GitHub volledig werkend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Onderzoek database verslag, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">verslag Steven, </t>
   </si>
 </sst>
 </file>
@@ -428,16 +440,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:E30"/>
+  <dimension ref="C4:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="89" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="89.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="97.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
@@ -458,7 +471,7 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
@@ -477,7 +490,7 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
@@ -485,7 +498,7 @@
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.25">
@@ -496,7 +509,7 @@
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
@@ -523,7 +536,7 @@
         <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
@@ -534,7 +547,7 @@
         <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
@@ -545,7 +558,7 @@
         <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
@@ -556,40 +569,69 @@
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E26" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
-        <v>41741</v>
+        <v>41771</v>
       </c>
       <c r="D28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" t="s">
         <v>23</v>
-      </c>
-      <c r="E28" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
-        <v>41742</v>
+        <v>41772</v>
+      </c>
+      <c r="D30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C32" s="1">
+        <v>41778</v>
+      </c>
+      <c r="D32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="1">
+        <v>41779</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="1">
+        <v>41785</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="1">
+        <v>41786</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="C26" twoDigitTextYear="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>